<commit_message>
changed the style of the file
</commit_message>
<xml_diff>
--- a/Contact_Hour_Worksheet.xlsx
+++ b/Contact_Hour_Worksheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Training\Project Management\PMI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\test\Hello-World\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B03A93-07C0-40DF-A40C-748591FC67F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ - Read Me First!" sheetId="2" r:id="rId1"/>
@@ -19,8 +20,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'FAQ - Read Me First!'!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,13 +39,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Home</author>
     <author>Kevin</author>
   </authors>
   <commentList>
-    <comment ref="G3" authorId="0" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="1" shapeId="0">
+    <comment ref="F12" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="1" shapeId="0">
+    <comment ref="F22" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="1" shapeId="0">
+    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -718,8 +728,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -799,20 +809,27 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0070C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -834,6 +851,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,7 +954,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1012,12 +1035,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1035,6 +1052,15 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1444,14 +1470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1462,10 +1488,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -1483,7 +1509,7 @@
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="42" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1584,8 +1610,8 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
     </row>
     <row r="22" spans="1:2" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
@@ -1594,8 +1620,8 @@
       <c r="B22" s="33"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1620,14 +1646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1645,34 +1671,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -1873,19 +1899,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39" t="s">
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
@@ -2054,19 +2080,19 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39" t="s">
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
@@ -2246,18 +2272,18 @@
       <c r="J33" s="29"/>
     </row>
     <row r="34" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
@@ -2283,7 +2309,7 @@
     <mergeCell ref="G23:J23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1"/>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="66" fitToHeight="99" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -2304,7 +2330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -2319,10 +2345,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="39"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
@@ -2433,12 +2459,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2" display="The PM PrepCast - A complete 35 hour PMP Workshop for your MP3 Player.."/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4" display="The PM Exam Simulator - 1,800 realistic sample questions…"/>
-    <hyperlink ref="B11" r:id="rId5" display="The PM Exam Simulator - 1,800 realistic sample questions…"/>
-    <hyperlink ref="B14" r:id="rId6" display="The PM Exam Simulator - 1,800 realistic sample questions…"/>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" display="The PM PrepCast - A complete 35 hour PMP Workshop for your MP3 Player.." xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B10" r:id="rId4" display="The PM Exam Simulator - 1,800 realistic sample questions…" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" display="The PM Exam Simulator - 1,800 realistic sample questions…" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" display="The PM Exam Simulator - 1,800 realistic sample questions…" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
added green to a column
</commit_message>
<xml_diff>
--- a/Contact_Hour_Worksheet.xlsx
+++ b/Contact_Hour_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\test\Hello-World\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B03A93-07C0-40DF-A40C-748591FC67F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC910ED9-3353-4812-94D0-97150CF591E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -829,7 +829,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +857,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,7 +960,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1060,6 +1066,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1477,7 +1486,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1521,7 +1530,7 @@
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="43" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>